<commit_message>
Added "log_molratio" unit. e.g for log(K/Na) in aqueous phase.
git-svn-id: svn+ssh://savannah01.psi.ch/repos/gems/GEMSFIT/branches/devGFshell@484 376c6ad0-4da0-11e1-87d0-276bdbf53620
</commit_message>
<xml_diff>
--- a/Tests/Aqueous/dbimport/Si-Na-K-Cl-OH.xlsx
+++ b/Tests/Aqueous/dbimport/Si-Na-K-Cl-OH.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="82" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="46" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -2094,28 +2094,29 @@
   <dimension ref="A1:AG49"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A22" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="AD8" activeCellId="0" pane="topLeft" sqref="AD8"/>
+      <selection activeCell="AD8" activeCellId="1" pane="topLeft" sqref="H394:P405 AD8"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.4666666666667"/>
-    <col collapsed="false" hidden="false" max="12" min="9" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="17.9607843137255"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="19.3529411764706"/>
-    <col collapsed="false" hidden="false" max="17" min="16" style="1" width="17.5372549019608"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="17.5372549019608"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.83529411764706"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="18.9372549019608"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="8.26666666666667"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.6627450980392"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.3764705882353"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.5725490196078"/>
-    <col collapsed="false" hidden="false" max="29" min="27" style="0" width="16"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="22.8745098039216"/>
-    <col collapsed="false" hidden="false" max="1025" min="32" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="7" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.5294117647059"/>
+    <col collapsed="false" hidden="false" max="12" min="9" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="18.0509803921569"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="1" width="19.4470588235294"/>
+    <col collapsed="false" hidden="false" max="17" min="16" style="1" width="17.6274509803922"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="17.6274509803922"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="8.88235294117647"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="8.54509803921569"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="19.0274509803922"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="8.30196078431373"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="10.7176470588235"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="18.4666666666667"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="15.6470588235294"/>
+    <col collapsed="false" hidden="false" max="29" min="27" style="0" width="16.0823529411765"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="0" width="22.9921568627451"/>
+    <col collapsed="false" hidden="false" max="1025" min="32" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="28.35" outlineLevel="0" r="1" s="4">
@@ -6112,28 +6113,28 @@
   </sheetPr>
   <dimension ref="A1:AC442"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A415" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B446" activeCellId="0" pane="topLeft" sqref="B446"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="D46" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="P394" activeCellId="0" pane="topLeft" sqref="H394:P405"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="10" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="10" width="31.9725490196078"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="12" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="10" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="10" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="22" min="14" style="10" width="16"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="10" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="10" width="18.243137254902"/>
-    <col collapsed="false" hidden="false" max="26" min="25" style="10" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="13" width="21.7529411764706"/>
-    <col collapsed="false" hidden="false" max="29" min="28" style="10" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="10" width="18.0980392156863"/>
-    <col collapsed="false" hidden="false" max="258" min="31" style="10" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="259" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="10" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="11" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="10" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="10" width="32.1333333333333"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="12" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="11" min="10" style="10" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="11" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="10" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="22" min="14" style="10" width="16.0823529411765"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="10" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="10" width="18.3333333333333"/>
+    <col collapsed="false" hidden="false" max="26" min="25" style="10" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="13" width="21.8588235294118"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="10" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="10" width="18.1882352941176"/>
+    <col collapsed="false" hidden="false" max="258" min="31" style="10" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="259" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="28.35" outlineLevel="0" r="1" s="17">
@@ -28032,7 +28033,7 @@
         <v>22</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="442">
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="442">
       <c r="A442" s="10" t="n">
         <v>441</v>
       </c>
@@ -28093,11 +28094,11 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="H394:P405 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="15.3" outlineLevel="0" r="1">

</xml_diff>